<commit_message>
Updated workout column to show A and B, and created date column
</commit_message>
<xml_diff>
--- a/NROL Basic Training 1.xlsx
+++ b/NROL Basic Training 1.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{C8DECFC4-1AA6-8F47-90A5-FD1B9B0432B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\danpa\Documents\Exercise\NROL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30499C6-FF4B-439E-9F8B-381F966624C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workout A" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
   <si>
     <t>Category</t>
   </si>
@@ -248,6 +252,15 @@
   </si>
   <si>
     <t>90 x 15</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -304,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -313,6 +326,10 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,7 +636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,20 +644,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7C7172-5154-A740-BD7F-8E2CBB3C6C81}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,8 +683,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -688,11 +709,14 @@
       <c r="G2" s="2">
         <v>30</v>
       </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -714,11 +738,14 @@
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -740,11 +767,14 @@
       <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -766,11 +796,14 @@
       <c r="G5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -792,11 +825,14 @@
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -818,11 +854,14 @@
       <c r="G7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -844,11 +883,14 @@
       <c r="G8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -868,11 +910,14 @@
         <v>43</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="5">
+        <v>44917</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H35" s="3"/>
     </row>
   </sheetData>
@@ -882,19 +927,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3244C7B-D9AB-C240-9447-20880B1BD5F9}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.43359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.8359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,8 +964,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -942,8 +990,14 @@
       <c r="G2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="5">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -965,8 +1019,14 @@
       <c r="G3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -988,8 +1048,14 @@
       <c r="G4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1011,8 +1077,14 @@
       <c r="G5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="5">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1034,8 +1106,14 @@
       <c r="G6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="5">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1057,8 +1135,14 @@
       <c r="G7">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="5">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1080,8 +1164,14 @@
       <c r="G8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="5">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1093,6 +1183,12 @@
       </c>
       <c r="D9" t="s">
         <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="5">
+        <v>44922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eliminated 2nd sheet and combined all information in one sheet
</commit_message>
<xml_diff>
--- a/NROL Basic Training 1.xlsx
+++ b/NROL Basic Training 1.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\danpa\Documents\Exercise\NROL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30499C6-FF4B-439E-9F8B-381F966624C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5383AAA8-19B0-4627-A8DA-B5B59BBC4A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workout A" sheetId="1" r:id="rId1"/>
-    <sheet name="Workout B" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Workout A'!$A$1:$I$17</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
   <si>
     <t>Category</t>
   </si>
@@ -189,12 +191,6 @@
   </si>
   <si>
     <t>pull</t>
-  </si>
-  <si>
-    <t>sets/reps</t>
-  </si>
-  <si>
-    <t>exercise</t>
   </si>
   <si>
     <t>2 x 30s</t>
@@ -317,18 +313,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -644,10 +637,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7C7172-5154-A740-BD7F-8E2CBB3C6C81}">
-  <dimension ref="A1:I35"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,8 +677,8 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>75</v>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -710,9 +704,9 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="5">
+        <v>71</v>
+      </c>
+      <c r="I2" s="4">
         <v>44917</v>
       </c>
     </row>
@@ -739,9 +733,9 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="5">
+        <v>71</v>
+      </c>
+      <c r="I3" s="4">
         <v>44917</v>
       </c>
     </row>
@@ -768,9 +762,9 @@
         <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="5">
+        <v>71</v>
+      </c>
+      <c r="I4" s="4">
         <v>44917</v>
       </c>
     </row>
@@ -797,9 +791,9 @@
         <v>27</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="5">
+        <v>71</v>
+      </c>
+      <c r="I5" s="4">
         <v>44917</v>
       </c>
     </row>
@@ -826,9 +820,9 @@
         <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" s="5">
+        <v>71</v>
+      </c>
+      <c r="I6" s="4">
         <v>44917</v>
       </c>
     </row>
@@ -855,9 +849,9 @@
         <v>35</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="5">
+        <v>71</v>
+      </c>
+      <c r="I7" s="4">
         <v>44917</v>
       </c>
     </row>
@@ -884,9 +878,9 @@
         <v>39</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="5">
+        <v>71</v>
+      </c>
+      <c r="I8" s="4">
         <v>44917</v>
       </c>
     </row>
@@ -911,287 +905,246 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="5">
+        <v>71</v>
+      </c>
+      <c r="I9" s="4">
         <v>44917</v>
       </c>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="3"/>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15">
+        <v>15</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="4">
+        <v>44922</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3244C7B-D9AB-C240-9447-20880B1BD5F9}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I5" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7">
-        <v>15</v>
-      </c>
-      <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" t="s">
-        <v>74</v>
-      </c>
-      <c r="I8" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="5">
-        <v>44922</v>
-      </c>
-    </row>
-  </sheetData>
+  <autoFilter ref="A1:I17" xr:uid="{3A7C7172-5154-A740-BD7F-8E2CBB3C6C81}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="A"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed NA's and left blanks instead.
</commit_message>
<xml_diff>
--- a/NROL Basic Training 1.xlsx
+++ b/NROL Basic Training 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\danpa\Documents\Exercise\NROL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5383AAA8-19B0-4627-A8DA-B5B59BBC4A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA16414-C780-4713-AC10-DE3E47CB3451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>Category</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Stability</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Plank</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
   </si>
   <si>
     <t>combo</t>
-  </si>
-  <si>
-    <t>na</t>
   </si>
   <si>
     <t>strength</t>
@@ -637,11 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7C7172-5154-A740-BD7F-8E2CBB3C6C81}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +671,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -688,14 +681,12 @@
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="2">
         <v>30</v>
@@ -704,7 +695,7 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I2" s="4">
         <v>44917</v>
@@ -715,25 +706,23 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I3" s="4">
         <v>44917</v>
@@ -741,28 +730,24 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I4" s="4">
         <v>44917</v>
@@ -770,28 +755,28 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I5" s="4">
         <v>44917</v>
@@ -799,28 +784,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I6" s="4">
         <v>44917</v>
@@ -828,28 +813,28 @@
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I7" s="4">
         <v>44917</v>
@@ -857,28 +842,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I8" s="4">
         <v>44917</v>
@@ -886,133 +871,117 @@
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I9" s="4">
         <v>44917</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I10" s="4">
         <v>44922</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
         <v>65</v>
       </c>
-      <c r="G11" t="s">
-        <v>67</v>
-      </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I11" s="4">
         <v>44922</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I12" s="4">
         <v>44922</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13">
         <v>15</v>
@@ -1021,27 +990,27 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I13" s="4">
         <v>44922</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -1050,27 +1019,27 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I14" s="4">
         <v>44922</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15">
         <v>15</v>
@@ -1079,56 +1048,50 @@
         <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I15" s="4">
         <v>44922</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" t="s">
         <v>70</v>
-      </c>
-      <c r="H16" t="s">
-        <v>72</v>
       </c>
       <c r="I16" s="4">
         <v>44922</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I17" s="4">
         <v>44922</v>
@@ -1138,13 +1101,7 @@
       <c r="H34" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I17" xr:uid="{3A7C7172-5154-A740-BD7F-8E2CBB3C6C81}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I17" xr:uid="{3A7C7172-5154-A740-BD7F-8E2CBB3C6C81}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>